<commit_message>
Implement new model to minimize the number of trips to go to the university. This works only if you allow more than 1 shift per day. Improve input parsing with argparse library.
</commit_message>
<xml_diff>
--- a/out/CSLibrary_Dec2018.xlsx
+++ b/out/CSLibrary_Dec2018.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="December 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="December 2018 Problem" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
-  <si>
-    <t>Automatic assignment for December 2018</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="22">
+  <si>
+    <t>Automatic assignment for December 2018 Problem</t>
   </si>
   <si>
     <t>Mon</t>
@@ -49,28 +49,31 @@
     <t>Giorgio</t>
   </si>
   <si>
+    <t>Libianchi Gabriele</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Filippo M</t>
+  </si>
+  <si>
+    <t>Utente Prova 2</t>
+  </si>
+  <si>
+    <t>Utente Prova</t>
+  </si>
+  <si>
+    <t>Andrea Coletta</t>
+  </si>
+  <si>
+    <t>Luigi Berducci</t>
+  </si>
+  <si>
+    <t>Piccola Ketty</t>
+  </si>
+  <si>
     <t>Alessandro</t>
-  </si>
-  <si>
-    <t>Andrea Coletta</t>
-  </si>
-  <si>
-    <t>Irene</t>
-  </si>
-  <si>
-    <t>Piccola Ketty</t>
-  </si>
-  <si>
-    <t>Libianchi Gabriele</t>
-  </si>
-  <si>
-    <t>Utente Prova</t>
-  </si>
-  <si>
-    <t>Filippo M</t>
-  </si>
-  <si>
-    <t>Luigi Berducci</t>
   </si>
   <si>
     <t>Student</t>
@@ -423,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,16 +488,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -505,16 +508,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -525,13 +528,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -556,19 +559,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -576,19 +579,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -596,13 +599,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -630,19 +633,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -650,19 +653,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -670,16 +673,16 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -704,19 +707,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -724,19 +727,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -744,16 +747,16 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -766,7 +769,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -774,7 +777,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -782,15 +785,15 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -806,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -822,7 +825,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -838,7 +841,7 @@
         <v>14</v>
       </c>
       <c r="B31" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -870,6 +873,14 @@
         <v>18</v>
       </c>
       <c r="B35" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="2">
         <v>6</v>
       </c>
     </row>

</xml_diff>